<commit_message>
Tag 10-4-2015 Workloads left:   - Test booking performance   - Change Promotion table, how to apply promotion in sale tab.   - Report
</commit_message>
<xml_diff>
--- a/SpaManagementV3/wiki/Maintenance Request.xlsx
+++ b/SpaManagementV3/wiki/Maintenance Request.xlsx
@@ -10,12 +10,12 @@
     <sheet name="Website" sheetId="1" r:id="rId1"/>
     <sheet name="Software" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="24">
   <si>
     <t>STT</t>
   </si>
@@ -47,15 +47,6 @@
     <t>Chỉnh sửa css</t>
   </si>
   <si>
-    <t>Thời lượng thực hiện</t>
-  </si>
-  <si>
-    <t>4.5 hours</t>
-  </si>
-  <si>
-    <t>3 hours</t>
-  </si>
-  <si>
     <t>29/1/2015</t>
   </si>
   <si>
@@ -85,23 +76,44 @@
     <t>13/2/2015</t>
   </si>
   <si>
-    <t>0.25 hours</t>
-  </si>
-  <si>
     <t>Thêm nội dung event cho site jp, chỉnh sửa lại format của các post event</t>
   </si>
   <si>
-    <t>4 hours</t>
+    <t>Fix mochuongspa@gmail.com run on outlook program (cant send and receive letter)</t>
+  </si>
+  <si>
+    <t>Sửa</t>
+  </si>
+  <si>
+    <t>Thời lượng thực hiện (giờ)</t>
+  </si>
+  <si>
+    <t>Tổng giờ</t>
+  </si>
+  <si>
+    <t>Đơn giá</t>
+  </si>
+  <si>
+    <t>Total</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="dd/mm/yyyy"/>
+  <numFmts count="3">
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="170" formatCode="[$-1010000]d/m/yyyy;@"/>
+    <numFmt numFmtId="175" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -127,8 +139,9 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -138,19 +151,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
+    <xf numFmtId="175" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="5">
     <dxf>
-      <numFmt numFmtId="164" formatCode="dd/mm/yyyy"/>
+      <numFmt numFmtId="170" formatCode="[$-1010000]d/m/yyyy;@"/>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -186,7 +198,7 @@
     <tableColumn id="2" name="Yêu cầu" dataDxfId="3"/>
     <tableColumn id="3" name="Loại yêu cầu" dataDxfId="2"/>
     <tableColumn id="4" name="Thời gian" dataDxfId="0"/>
-    <tableColumn id="5" name="Thời lượng thực hiện" dataDxfId="1"/>
+    <tableColumn id="5" name="Thời lượng thực hiện (giờ)" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight11" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -491,10 +503,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:F24"/>
+  <dimension ref="B2:J24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -504,9 +516,11 @@
     <col min="4" max="4" width="17.88671875" style="1" customWidth="1"/>
     <col min="5" max="5" width="13.21875" style="3" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="23" style="1" customWidth="1"/>
+    <col min="9" max="9" width="11.109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
         <v>0</v>
       </c>
@@ -520,10 +534,19 @@
         <v>2</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="3" spans="2:6" ht="86.4" x14ac:dyDescent="0.3">
+        <v>20</v>
+      </c>
+      <c r="H2" t="s">
+        <v>21</v>
+      </c>
+      <c r="I2" t="s">
+        <v>22</v>
+      </c>
+      <c r="J2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="3" spans="2:10" ht="86.4" x14ac:dyDescent="0.3">
       <c r="B3" s="1">
         <v>1</v>
       </c>
@@ -534,13 +557,24 @@
         <v>5</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="4" spans="2:6" ht="43.2" x14ac:dyDescent="0.3">
+        <v>10</v>
+      </c>
+      <c r="F3" s="1">
+        <v>4.5</v>
+      </c>
+      <c r="H3">
+        <f>SUM(F3:F18)</f>
+        <v>21.75</v>
+      </c>
+      <c r="I3" s="4">
+        <v>50000</v>
+      </c>
+      <c r="J3" s="4">
+        <f>H3*I3</f>
+        <v>1087500</v>
+      </c>
+    </row>
+    <row r="4" spans="2:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B4" s="1">
         <v>2</v>
       </c>
@@ -551,116 +585,130 @@
         <v>7</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
+        <v>8</v>
+      </c>
+      <c r="F4" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="2:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B5" s="1">
         <v>3</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E5" s="4">
+        <v>9</v>
+      </c>
+      <c r="E5" s="3">
         <v>42065</v>
       </c>
-      <c r="F5" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="6" spans="2:6" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="F5" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="2:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B6" s="1">
         <v>4</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="E6" s="4">
+        <v>12</v>
+      </c>
+      <c r="E6" s="3">
         <v>42126</v>
       </c>
-      <c r="F6" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="7" spans="2:6" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="F6" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="2:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B7" s="1">
         <v>5</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="E7" s="4">
+        <v>12</v>
+      </c>
+      <c r="E7" s="3">
         <v>42126</v>
       </c>
-      <c r="F7" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="8" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="F7" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B8" s="1">
         <v>6</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="9" spans="2:6" x14ac:dyDescent="0.3">
+        <v>16</v>
+      </c>
+      <c r="F8" s="1">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="9" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B9" s="1">
         <v>7</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>5</v>
       </c>
       <c r="E9" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F9" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B10" s="1"/>
+    </row>
+    <row r="11" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B11" s="1">
+        <v>8</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D11" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="F9" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="10" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B10" s="1"/>
-    </row>
-    <row r="11" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B11" s="1"/>
-    </row>
-    <row r="12" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="E11" s="3">
+        <v>42281</v>
+      </c>
+      <c r="F11" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B12" s="1"/>
     </row>
-    <row r="13" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B13" s="1"/>
     </row>
-    <row r="14" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B14" s="1"/>
     </row>
-    <row r="15" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B15" s="1"/>
     </row>
-    <row r="16" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B16" s="1"/>
     </row>
     <row r="17" spans="2:2" x14ac:dyDescent="0.3">

</xml_diff>